<commit_message>
Add intro to dplyr script
</commit_message>
<xml_diff>
--- a/data_raw/messy_data.xlsx
+++ b/data_raw/messy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30257d98913de859/GitHub/teaching/CBC_R_club/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ED2EBF6-0830-4C6E-809D-0BC5055ED6D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{9ED2EBF6-0830-4C6E-809D-0BC5055ED6D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8A6B371B-EC40-4B8A-B621-41C2AEE6F3C8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3186B349-B455-43FE-9772-D0DB154C9E98}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,7 +483,7 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>